<commit_message>
init data and read data from excel
</commit_message>
<xml_diff>
--- a/initData.xlsx
+++ b/initData.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\apache\Apache24\htdocs\php\SubjectSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D286E0B-9F61-49FF-A95E-E350FEB07456}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA81959-D037-4091-AAFD-D8550FB93712}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classroom" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="238">
   <si>
     <t>A001</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -889,6 +889,78 @@
   </si>
   <si>
     <t>About the topic of the lecture</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>classroom_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>capacity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>time_slot_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>start_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>end_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>day_of_week</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>course_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>course_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>credit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>class_hours</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instructor_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instructor_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hire_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>quit_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exam_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>week</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>demand</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -897,7 +969,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -945,7 +1017,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1227,25 +1299,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>50</v>
+        <v>220</v>
+      </c>
+      <c r="B1" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>50</v>
@@ -1253,63 +1326,63 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>209</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>209</v>
       </c>
       <c r="B8">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>100</v>
@@ -1317,7 +1390,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>100</v>
@@ -1325,7 +1398,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
       <c r="B12">
         <v>100</v>
@@ -1333,24 +1406,34 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13">
         <v>100</v>
       </c>
-      <c r="B13">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1D7907-68E8-4DD9-809E-4A1EA7430963}">
-  <dimension ref="A1:B1"/>
+  <sheetPr codeName="Sheet10"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -1360,9 +1443,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
         <v>216</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>219</v>
       </c>
     </row>
@@ -1374,10 +1465,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC06F30-D5F5-418E-903B-674DDAE55723}">
-  <dimension ref="A1:D60"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -1387,27 +1479,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C1" s="1">
-        <v>0.36458333333333331</v>
-      </c>
-      <c r="D1">
-        <v>1</v>
+        <v>222</v>
+      </c>
+      <c r="B1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1">
-        <v>0.37152777777777773</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C2" s="1">
-        <v>0.40277777777777773</v>
+        <v>0.36458333333333331</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1415,13 +1507,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
-        <v>0.41319444444444442</v>
+        <v>0.37152777777777773</v>
       </c>
       <c r="C3" s="1">
-        <v>0.44444444444444442</v>
+        <v>0.40277777777777773</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1429,13 +1521,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1">
-        <v>0.4513888888888889</v>
+        <v>0.41319444444444442</v>
       </c>
       <c r="C4" s="1">
-        <v>0.4826388888888889</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1443,13 +1535,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
-        <v>0.48958333333333331</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="C5" s="1">
-        <v>0.52083333333333337</v>
+        <v>0.4826388888888889</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1457,13 +1549,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1">
-        <v>0.5625</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="C6" s="1">
-        <v>0.59375</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1471,13 +1563,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1">
-        <v>0.60069444444444442</v>
+        <v>0.5625</v>
       </c>
       <c r="C7" s="1">
-        <v>0.63194444444444442</v>
+        <v>0.59375</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1485,13 +1577,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1">
-        <v>0.64236111111111105</v>
+        <v>0.60069444444444442</v>
       </c>
       <c r="C8" s="1">
-        <v>0.67361111111111116</v>
+        <v>0.63194444444444442</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1499,13 +1591,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1">
-        <v>0.68402777777777779</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.71527777777777779</v>
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.67361111111111116</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1513,13 +1605,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.80208333333333337</v>
+        <v>0.68402777777777779</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.71527777777777779</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1527,13 +1619,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1">
-        <v>0.80902777777777779</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="C11" s="1">
-        <v>0.84027777777777779</v>
+        <v>0.80208333333333337</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1541,13 +1633,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1">
-        <v>0.85069444444444453</v>
+        <v>0.80902777777777779</v>
       </c>
       <c r="C12" s="1">
-        <v>0.88194444444444453</v>
+        <v>0.84027777777777779</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1555,27 +1647,27 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.85069444444444453</v>
       </c>
       <c r="C13" s="1">
-        <v>0.36458333333333331</v>
+        <v>0.88194444444444453</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1">
-        <v>0.37152777777777773</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C14" s="1">
-        <v>0.40277777777777773</v>
+        <v>0.36458333333333331</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -1583,13 +1675,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1">
-        <v>0.41319444444444442</v>
+        <v>0.37152777777777773</v>
       </c>
       <c r="C15" s="1">
-        <v>0.44444444444444442</v>
+        <v>0.40277777777777773</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -1597,13 +1689,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1">
-        <v>0.4513888888888889</v>
+        <v>0.41319444444444442</v>
       </c>
       <c r="C16" s="1">
-        <v>0.4826388888888889</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1611,13 +1703,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1">
-        <v>0.48958333333333331</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="C17" s="1">
-        <v>0.52083333333333337</v>
+        <v>0.4826388888888889</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -1625,13 +1717,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1">
-        <v>0.5625</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="C18" s="1">
-        <v>0.59375</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -1639,13 +1731,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="1">
-        <v>0.60069444444444442</v>
+        <v>0.5625</v>
       </c>
       <c r="C19" s="1">
-        <v>0.63194444444444442</v>
+        <v>0.59375</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -1653,13 +1745,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1">
-        <v>0.64236111111111105</v>
+        <v>0.60069444444444442</v>
       </c>
       <c r="C20" s="1">
-        <v>0.67361111111111116</v>
+        <v>0.63194444444444442</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -1667,13 +1759,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="1">
-        <v>0.68402777777777779</v>
-      </c>
-      <c r="C21" s="2">
-        <v>0.71527777777777779</v>
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.67361111111111116</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -1681,13 +1773,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="1">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0.80208333333333337</v>
+        <v>0.68402777777777779</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.71527777777777779</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -1695,13 +1787,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="1">
-        <v>0.80902777777777779</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="C23" s="1">
-        <v>0.84027777777777779</v>
+        <v>0.80208333333333337</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -1709,13 +1801,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="1">
-        <v>0.85069444444444453</v>
+        <v>0.80902777777777779</v>
       </c>
       <c r="C24" s="1">
-        <v>0.88194444444444453</v>
+        <v>0.84027777777777779</v>
       </c>
       <c r="D24">
         <v>2</v>
@@ -1723,27 +1815,27 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.85069444444444453</v>
       </c>
       <c r="C25" s="1">
-        <v>0.36458333333333331</v>
+        <v>0.88194444444444453</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1">
-        <v>0.37152777777777773</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C26" s="1">
-        <v>0.40277777777777773</v>
+        <v>0.36458333333333331</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -1751,13 +1843,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1">
-        <v>0.41319444444444442</v>
+        <v>0.37152777777777773</v>
       </c>
       <c r="C27" s="1">
-        <v>0.44444444444444442</v>
+        <v>0.40277777777777773</v>
       </c>
       <c r="D27">
         <v>3</v>
@@ -1765,13 +1857,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" s="1">
-        <v>0.4513888888888889</v>
+        <v>0.41319444444444442</v>
       </c>
       <c r="C28" s="1">
-        <v>0.4826388888888889</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="D28">
         <v>3</v>
@@ -1779,13 +1871,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" s="1">
-        <v>0.48958333333333331</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="C29" s="1">
-        <v>0.52083333333333337</v>
+        <v>0.4826388888888889</v>
       </c>
       <c r="D29">
         <v>3</v>
@@ -1793,13 +1885,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" s="1">
-        <v>0.5625</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="C30" s="1">
-        <v>0.59375</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -1807,13 +1899,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B31" s="1">
-        <v>0.60069444444444442</v>
+        <v>0.5625</v>
       </c>
       <c r="C31" s="1">
-        <v>0.63194444444444442</v>
+        <v>0.59375</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -1821,13 +1913,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" s="1">
-        <v>0.64236111111111105</v>
+        <v>0.60069444444444442</v>
       </c>
       <c r="C32" s="1">
-        <v>0.67361111111111116</v>
+        <v>0.63194444444444442</v>
       </c>
       <c r="D32">
         <v>3</v>
@@ -1835,13 +1927,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B33" s="1">
-        <v>0.68402777777777779</v>
-      </c>
-      <c r="C33" s="2">
-        <v>0.71527777777777779</v>
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.67361111111111116</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -1849,13 +1941,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B34" s="1">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="C34" s="1">
-        <v>0.80208333333333337</v>
+        <v>0.68402777777777779</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.71527777777777779</v>
       </c>
       <c r="D34">
         <v>3</v>
@@ -1863,13 +1955,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B35" s="1">
-        <v>0.80902777777777779</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="C35" s="1">
-        <v>0.84027777777777779</v>
+        <v>0.80208333333333337</v>
       </c>
       <c r="D35">
         <v>3</v>
@@ -1877,13 +1969,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B36" s="1">
-        <v>0.85069444444444453</v>
+        <v>0.80902777777777779</v>
       </c>
       <c r="C36" s="1">
-        <v>0.88194444444444453</v>
+        <v>0.84027777777777779</v>
       </c>
       <c r="D36">
         <v>3</v>
@@ -1891,27 +1983,27 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B37" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.85069444444444453</v>
       </c>
       <c r="C37" s="1">
-        <v>0.36458333333333331</v>
+        <v>0.88194444444444453</v>
       </c>
       <c r="D37">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B38" s="1">
-        <v>0.37152777777777773</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C38" s="1">
-        <v>0.40277777777777773</v>
+        <v>0.36458333333333331</v>
       </c>
       <c r="D38">
         <v>4</v>
@@ -1919,13 +2011,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B39" s="1">
-        <v>0.41319444444444442</v>
+        <v>0.37152777777777773</v>
       </c>
       <c r="C39" s="1">
-        <v>0.44444444444444442</v>
+        <v>0.40277777777777773</v>
       </c>
       <c r="D39">
         <v>4</v>
@@ -1933,13 +2025,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B40" s="1">
-        <v>0.4513888888888889</v>
+        <v>0.41319444444444442</v>
       </c>
       <c r="C40" s="1">
-        <v>0.4826388888888889</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="D40">
         <v>4</v>
@@ -1947,13 +2039,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B41" s="1">
-        <v>0.48958333333333331</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="C41" s="1">
-        <v>0.52083333333333337</v>
+        <v>0.4826388888888889</v>
       </c>
       <c r="D41">
         <v>4</v>
@@ -1961,13 +2053,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B42" s="1">
-        <v>0.5625</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="C42" s="1">
-        <v>0.59375</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="D42">
         <v>4</v>
@@ -1975,13 +2067,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B43" s="1">
-        <v>0.60069444444444442</v>
+        <v>0.5625</v>
       </c>
       <c r="C43" s="1">
-        <v>0.63194444444444442</v>
+        <v>0.59375</v>
       </c>
       <c r="D43">
         <v>4</v>
@@ -1989,13 +2081,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B44" s="1">
-        <v>0.64236111111111105</v>
+        <v>0.60069444444444442</v>
       </c>
       <c r="C44" s="1">
-        <v>0.67361111111111116</v>
+        <v>0.63194444444444442</v>
       </c>
       <c r="D44">
         <v>4</v>
@@ -2003,13 +2095,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B45" s="1">
-        <v>0.68402777777777779</v>
-      </c>
-      <c r="C45" s="2">
-        <v>0.71527777777777779</v>
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0.67361111111111116</v>
       </c>
       <c r="D45">
         <v>4</v>
@@ -2017,13 +2109,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B46" s="1">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="C46" s="1">
-        <v>0.80208333333333337</v>
+        <v>0.68402777777777779</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.71527777777777779</v>
       </c>
       <c r="D46">
         <v>4</v>
@@ -2031,13 +2123,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B47" s="1">
-        <v>0.80902777777777779</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="C47" s="1">
-        <v>0.84027777777777779</v>
+        <v>0.80208333333333337</v>
       </c>
       <c r="D47">
         <v>4</v>
@@ -2045,13 +2137,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B48" s="1">
-        <v>0.85069444444444453</v>
+        <v>0.80902777777777779</v>
       </c>
       <c r="C48" s="1">
-        <v>0.88194444444444453</v>
+        <v>0.84027777777777779</v>
       </c>
       <c r="D48">
         <v>4</v>
@@ -2059,27 +2151,27 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B49" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.85069444444444453</v>
       </c>
       <c r="C49" s="1">
-        <v>0.36458333333333331</v>
+        <v>0.88194444444444453</v>
       </c>
       <c r="D49">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B50" s="1">
-        <v>0.37152777777777773</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C50" s="1">
-        <v>0.40277777777777773</v>
+        <v>0.36458333333333331</v>
       </c>
       <c r="D50">
         <v>5</v>
@@ -2087,13 +2179,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B51" s="1">
-        <v>0.41319444444444442</v>
+        <v>0.37152777777777773</v>
       </c>
       <c r="C51" s="1">
-        <v>0.44444444444444442</v>
+        <v>0.40277777777777773</v>
       </c>
       <c r="D51">
         <v>5</v>
@@ -2101,13 +2193,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B52" s="1">
-        <v>0.4513888888888889</v>
+        <v>0.41319444444444442</v>
       </c>
       <c r="C52" s="1">
-        <v>0.4826388888888889</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="D52">
         <v>5</v>
@@ -2115,13 +2207,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B53" s="1">
-        <v>0.48958333333333331</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="C53" s="1">
-        <v>0.52083333333333337</v>
+        <v>0.4826388888888889</v>
       </c>
       <c r="D53">
         <v>5</v>
@@ -2129,13 +2221,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B54" s="1">
-        <v>0.5625</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="C54" s="1">
-        <v>0.59375</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="D54">
         <v>5</v>
@@ -2143,13 +2235,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A55" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B55" s="1">
-        <v>0.60069444444444442</v>
+        <v>0.5625</v>
       </c>
       <c r="C55" s="1">
-        <v>0.63194444444444442</v>
+        <v>0.59375</v>
       </c>
       <c r="D55">
         <v>5</v>
@@ -2157,13 +2249,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B56" s="1">
-        <v>0.64236111111111105</v>
+        <v>0.60069444444444442</v>
       </c>
       <c r="C56" s="1">
-        <v>0.67361111111111116</v>
+        <v>0.63194444444444442</v>
       </c>
       <c r="D56">
         <v>5</v>
@@ -2171,13 +2263,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B57" s="1">
-        <v>0.68402777777777779</v>
-      </c>
-      <c r="C57" s="2">
-        <v>0.71527777777777779</v>
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0.67361111111111116</v>
       </c>
       <c r="D57">
         <v>5</v>
@@ -2185,13 +2277,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B58" s="1">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="C58" s="1">
-        <v>0.80208333333333337</v>
+        <v>0.68402777777777779</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0.71527777777777779</v>
       </c>
       <c r="D58">
         <v>5</v>
@@ -2199,13 +2291,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B59" s="1">
-        <v>0.80902777777777779</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="C59" s="1">
-        <v>0.84027777777777779</v>
+        <v>0.80208333333333337</v>
       </c>
       <c r="D59">
         <v>5</v>
@@ -2213,15 +2305,29 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A60" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="C60" s="1">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="D60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A61" t="s">
         <v>71</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B61" s="1">
         <v>0.85069444444444453</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C61" s="1">
         <v>0.88194444444444453</v>
       </c>
-      <c r="D60">
+      <c r="D61">
         <v>5</v>
       </c>
     </row>
@@ -2233,10 +2339,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623BDB94-C9AC-4CE7-96C3-30EFE8D45771}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -3090,10 +3197,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C33A3026-BB90-4E32-A3D3-57B88F0CF511}">
-  <dimension ref="A1:D19"/>
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -3103,80 +3211,80 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>226</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1">
-        <v>4</v>
-      </c>
-      <c r="D1">
-        <v>64</v>
+        <v>227</v>
+      </c>
+      <c r="C1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>80</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
         <v>80</v>
-      </c>
-      <c r="B5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -3187,10 +3295,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -3201,52 +3309,52 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>64</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -3257,10 +3365,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -3271,66 +3379,66 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D13">
-        <v>32</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D15">
-        <v>64</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D16">
-        <v>16</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -3341,29 +3449,43 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A20" t="s">
         <v>11</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>104</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>3</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <v>48</v>
       </c>
     </row>
@@ -3376,10 +3498,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{014C9AFD-5534-4BBD-B3BD-29FE9EE0F54D}">
-  <dimension ref="A1:D15"/>
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -3390,27 +3513,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>230</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C1" s="3">
-        <v>39479</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>122</v>
+        <v>231</v>
+      </c>
+      <c r="C1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="C2" s="3">
-        <v>35132</v>
+        <v>39479</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>122</v>
@@ -3418,13 +3541,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="C3" s="3">
-        <v>36448</v>
+        <v>35132</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>122</v>
@@ -3432,13 +3555,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C4" s="3">
-        <v>43586</v>
+        <v>36448</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>122</v>
@@ -3446,13 +3569,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B5" t="s">
-        <v>202</v>
+        <v>130</v>
       </c>
       <c r="C5" s="3">
-        <v>38976</v>
+        <v>43586</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>122</v>
@@ -3460,13 +3583,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>202</v>
       </c>
       <c r="C6" s="3">
-        <v>32883</v>
+        <v>38976</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>122</v>
@@ -3474,13 +3597,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C7" s="3">
-        <v>36962</v>
+        <v>32883</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>122</v>
@@ -3488,27 +3611,27 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C8" s="3">
-        <v>40275</v>
+        <v>36962</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C9" s="3">
-        <v>41834</v>
+        <v>40275</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>128</v>
@@ -3516,13 +3639,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C10" s="3">
-        <v>32512</v>
+        <v>41834</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>128</v>
@@ -3530,13 +3653,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C11" s="3">
-        <v>43399</v>
+        <v>32512</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>128</v>
@@ -3544,13 +3667,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C12" s="3">
-        <v>40045</v>
+        <v>43399</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>128</v>
@@ -3558,23 +3681,37 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" s="3">
+        <v>40045</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
         <v>139</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>140</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C14" s="3">
         <v>39519</v>
       </c>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.5">
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3584,6 +3721,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499D8A3C-FCAC-499A-93D3-FD4E015A34E8}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3906,6 +4044,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15B8C0D-B99E-425E-9B8D-563199920B79}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3919,25 +4058,26 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DEF9D93-ABFD-4958-B6AE-25C62304BD5B}">
-  <dimension ref="A1:B18"/>
+  <sheetPr codeName="Sheet8"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B1">
-        <v>17</v>
+        <v>234</v>
+      </c>
+      <c r="B1" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2">
         <v>17</v>
@@ -3945,7 +4085,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B3">
         <v>17</v>
@@ -3953,7 +4093,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B4">
         <v>17</v>
@@ -3961,7 +4101,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B5">
         <v>17</v>
@@ -3969,7 +4109,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B6">
         <v>17</v>
@@ -3977,7 +4117,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B7">
         <v>17</v>
@@ -3985,7 +4125,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B8">
         <v>17</v>
@@ -3993,7 +4133,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9">
         <v>17</v>
@@ -4001,7 +4141,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B10">
         <v>17</v>
@@ -4009,7 +4149,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B11">
         <v>17</v>
@@ -4017,7 +4157,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B12">
         <v>17</v>
@@ -4025,7 +4165,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B13">
         <v>17</v>
@@ -4033,7 +4173,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B14">
         <v>17</v>
@@ -4041,7 +4181,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B15">
         <v>17</v>
@@ -4049,7 +4189,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B16">
         <v>17</v>
@@ -4057,7 +4197,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B17">
         <v>17</v>
@@ -4065,9 +4205,17 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
+        <v>187</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
         <v>188</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>17</v>
       </c>
     </row>
@@ -4079,10 +4227,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6A4684C-55C5-4398-82FD-B3C96D999242}">
-  <dimension ref="A1:B17"/>
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -4092,31 +4241,31 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>217</v>
+        <v>234</v>
+      </c>
+      <c r="B1" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>217</v>
@@ -4124,23 +4273,23 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>217</v>
@@ -4148,7 +4297,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>217</v>
@@ -4156,7 +4305,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>217</v>
@@ -4164,23 +4313,23 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>217</v>
@@ -4188,7 +4337,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>217</v>
@@ -4196,7 +4345,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>217</v>
@@ -4204,7 +4353,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>217</v>
@@ -4212,7 +4361,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>217</v>
@@ -4220,9 +4369,17 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
         <v>188</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>217</v>
       </c>
     </row>

</xml_diff>